<commit_message>
fixing predict checkValidFile case
</commit_message>
<xml_diff>
--- a/data/RealData/full_genomeid_classification.xlsx
+++ b/data/RealData/full_genomeid_classification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/celsloaner/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagoyal/Documents/kb_genomeclassification/data/RealData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ADDE4D0-E88C-D34A-BE59-FB6EA36D71E2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D284CA-41A3-0643-8E65-63949B578C9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{9D33719E-AF2C-C846-B800-8BB48A352A14}"/>
+    <workbookView xWindow="3240" yWindow="5820" windowWidth="25440" windowHeight="15000" xr2:uid="{9D33719E-AF2C-C846-B800-8BB48A352A14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,17 @@
     <t>facultative</t>
   </si>
   <si>
-    <t>Genome_ID</t>
+    <t>Genome Name</t>
   </si>
   <si>
-    <t>Classification</t>
+    <t>Phenotype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -394,16 +394,16 @@
   <dimension ref="A1:B291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -411,7 +411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>204669.6</v>
       </c>
@@ -419,7 +419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>234267.13</v>
       </c>
@@ -427,7 +427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>240015.3</v>
       </c>
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>1806.1</v>
       </c>
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>83331.100000000006</v>
       </c>
@@ -451,7 +451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>106370.11</v>
       </c>
@@ -459,7 +459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>164756.6</v>
       </c>
@@ -467,7 +467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>196627.4</v>
       </c>
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>216594.1</v>
       </c>
@@ -483,7 +483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>227882.1</v>
       </c>
@@ -491,7 +491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>233413.1</v>
       </c>
@@ -499,7 +499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>246196.1</v>
       </c>
@@ -507,7 +507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>262316.09999999998</v>
       </c>
@@ -515,7 +515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>266117.59999999998</v>
       </c>
@@ -523,7 +523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>272631.09999999998</v>
       </c>
@@ -531,7 +531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>313589.3</v>
       </c>
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>321955.40000000002</v>
       </c>
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>350058.5</v>
       </c>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>351607.5</v>
       </c>
@@ -563,7 +563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>369723.3</v>
       </c>
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>391037.3</v>
       </c>
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>443906.13</v>
       </c>
@@ -587,7 +587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>446470.40000000002</v>
       </c>
@@ -595,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>471857.4</v>
       </c>
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>479431.5</v>
       </c>
@@ -611,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>526225.5</v>
       </c>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>698972.3</v>
       </c>
@@ -627,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>994479.3</v>
       </c>
@@ -635,7 +635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>1146883.3</v>
       </c>
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>1206734.3999999999</v>
       </c>
@@ -651,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>1206739.3999999999</v>
       </c>
@@ -659,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>469378.5</v>
       </c>
@@ -667,7 +667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>518634.7</v>
       </c>
@@ -675,7 +675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>722911.3</v>
       </c>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>866770.3</v>
       </c>
@@ -691,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>435830.3</v>
       </c>
@@ -699,7 +699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>879307.3</v>
       </c>
@@ -707,7 +707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>783.1</v>
       </c>
@@ -715,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>955.1</v>
       </c>
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>35793.1</v>
       </c>
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>48935.1</v>
       </c>
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>52598.3</v>
       </c>
@@ -747,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>190650.1</v>
       </c>
@@ -755,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>204722.1</v>
       </c>
@@ -763,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>205920.8</v>
       </c>
@@ -771,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>212042.5</v>
       </c>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>216596.1</v>
       </c>
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>224911.1</v>
       </c>
@@ -795,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>224914.1</v>
       </c>
@@ -803,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>228405.5</v>
       </c>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>234826.3</v>
       </c>
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>237727.3</v>
       </c>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>246200.3</v>
       </c>
@@ -835,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>252305.3</v>
       </c>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>254945.3</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>257363.1</v>
       </c>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>262698.3</v>
       </c>
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2">
       <c r="A59">
         <v>264203.3</v>
       </c>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2">
       <c r="A60">
         <v>266779.09999999998</v>
       </c>
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2">
       <c r="A61">
         <v>266834.09999999998</v>
       </c>
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2">
       <c r="A62">
         <v>266835.09999999998</v>
       </c>
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2">
       <c r="A63">
         <v>269484.40000000002</v>
       </c>
@@ -907,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2">
       <c r="A64">
         <v>272944.09999999998</v>
       </c>
@@ -915,7 +915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>272947.09999999998</v>
       </c>
@@ -923,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>288000.5</v>
       </c>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2">
       <c r="A67">
         <v>290633.09999999998</v>
       </c>
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2">
       <c r="A68">
         <v>292414.09999999998</v>
       </c>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2">
       <c r="A69">
         <v>292805.3</v>
       </c>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2">
       <c r="A70">
         <v>293614.3</v>
       </c>
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2">
       <c r="A71">
         <v>314225.3</v>
       </c>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2">
       <c r="A72">
         <v>314232.3</v>
       </c>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2">
       <c r="A73">
         <v>314254.3</v>
       </c>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2">
       <c r="A74">
         <v>314260.3</v>
       </c>
@@ -995,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2">
       <c r="A75">
         <v>315456.3</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2">
       <c r="A76">
         <v>317655.90000000002</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2">
       <c r="A77">
         <v>318586.40000000002</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2">
       <c r="A78">
         <v>335992.3</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2">
       <c r="A79">
         <v>336407.4</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2">
       <c r="A80">
         <v>342108.5</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2">
       <c r="A81">
         <v>349163.4</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2">
       <c r="A82">
         <v>360095.3</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2">
       <c r="A83">
         <v>366602.3</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2">
       <c r="A84">
         <v>391165.8</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2">
       <c r="A85">
         <v>392499.4</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2">
       <c r="A86">
         <v>394221.5</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2">
       <c r="A87">
         <v>402881.6</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2">
       <c r="A88">
         <v>419610.8</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2">
       <c r="A89">
         <v>426117.3</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2">
       <c r="A90">
         <v>431944.4</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2">
       <c r="A91">
         <v>483179.3</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2">
       <c r="A92">
         <v>1112213.3</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2">
       <c r="A93">
         <v>398580.3</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2">
       <c r="A94">
         <v>224324.1</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2">
       <c r="A95">
         <v>648996.5</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2">
       <c r="A96">
         <v>868864.3</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2">
       <c r="A97">
         <v>66692.3</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2">
       <c r="A98">
         <v>93061.3</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2">
       <c r="A99">
         <v>176279.3</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2">
       <c r="A100">
         <v>220668.1</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2">
       <c r="A101">
         <v>224308.1</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2">
       <c r="A102">
         <v>235909.3</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2">
       <c r="A103">
         <v>257314.1</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2">
       <c r="A104">
         <v>272558.09999999998</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2">
       <c r="A105">
         <v>272621.3</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2">
       <c r="A106">
         <v>279010.5</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2">
       <c r="A107">
         <v>279808.3</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2">
       <c r="A108">
         <v>281309.3</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2">
       <c r="A109">
         <v>299033.59999999998</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2">
       <c r="A110">
         <v>315730.5</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2">
       <c r="A111">
         <v>321956.5</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2">
       <c r="A112">
         <v>321967.8</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2">
       <c r="A113">
         <v>342451.4</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2">
       <c r="A114">
         <v>387344.13</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2">
       <c r="A115">
         <v>405566.3</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2">
       <c r="A116">
         <v>420246.5</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2">
       <c r="A117">
         <v>169963.1</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2">
       <c r="A118">
         <v>272626.09999999998</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2">
       <c r="A119">
         <v>386043.6</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2">
       <c r="A120">
         <v>262543.40000000002</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2">
       <c r="A121">
         <v>1134785.3</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2">
       <c r="A122">
         <v>216432.3</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2">
       <c r="A123">
         <v>269798.12</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2">
       <c r="A124">
         <v>309807.19</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2">
       <c r="A125">
         <v>411154.5</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2">
       <c r="A126">
         <v>485917.5</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2">
       <c r="A127">
         <v>485918.5</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2">
       <c r="A128">
         <v>457391.3</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2">
       <c r="A129">
         <v>470145.6</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2">
       <c r="A130">
         <v>665954.30000000005</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2">
       <c r="A131">
         <v>679190.3</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2">
       <c r="A132">
         <v>702438.40000000002</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2">
       <c r="A133">
         <v>752555.5</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2">
       <c r="A134">
         <v>997879.3</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2">
       <c r="A135">
         <v>997891.3</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2">
       <c r="A136">
         <v>1042376.3</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2">
       <c r="A137">
         <v>376686.6</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2">
       <c r="A138">
         <v>402612.4</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2">
       <c r="A139">
         <v>486.1</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2">
       <c r="A140">
         <v>487.2</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2">
       <c r="A141">
         <v>36873.1</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2">
       <c r="A142">
         <v>76114.399999999994</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2">
       <c r="A143">
         <v>204773.3</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2">
       <c r="A144">
         <v>216591.1</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2">
       <c r="A145">
         <v>228410.1</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2">
       <c r="A146">
         <v>232721.5</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2">
       <c r="A147">
         <v>243160.4</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2">
       <c r="A148">
         <v>243365.1</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2">
       <c r="A149">
         <v>264198.3</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2">
       <c r="A150">
         <v>265072.7</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2">
       <c r="A151">
         <v>266264.40000000002</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2">
       <c r="A152">
         <v>267608.09999999998</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2">
       <c r="A153">
         <v>272560.3</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2">
       <c r="A154">
         <v>292415.3</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2">
       <c r="A155">
         <v>296591.09999999998</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2">
       <c r="A156">
         <v>335283.5</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2">
       <c r="A157">
         <v>339670.3</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2">
       <c r="A158">
         <v>350701.3</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2">
       <c r="A159">
         <v>391735.5</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2">
       <c r="A160">
         <v>395019.3</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2">
       <c r="A161">
         <v>395495.3</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2">
       <c r="A162">
         <v>398578.3</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2">
       <c r="A163">
         <v>999394.3</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2">
       <c r="A164">
         <v>115711.7</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2">
       <c r="A165">
         <v>218497.4</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2">
       <c r="A166">
         <v>227941.1</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2">
       <c r="A167">
         <v>243161.4</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2">
       <c r="A168">
         <v>264202.3</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2">
       <c r="A169">
         <v>759364.3</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2">
       <c r="A170">
         <v>194439.7</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2">
       <c r="A171">
         <v>517417.4</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2">
       <c r="A172">
         <v>316274.3</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2">
       <c r="A173">
         <v>324602.8</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2">
       <c r="A174">
         <v>383372.4</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2">
       <c r="A175">
         <v>292459.09999999998</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2">
       <c r="A176">
         <v>1496.1</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2">
       <c r="A177">
         <v>138119.29999999999</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2">
       <c r="A178">
         <v>195102.1</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2">
       <c r="A179">
         <v>203119.1</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2">
       <c r="A180">
         <v>212717.1</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2">
       <c r="A181">
         <v>246194.3</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2">
       <c r="A182">
         <v>264732.90000000002</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2">
       <c r="A183">
         <v>290402.34000000003</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2">
       <c r="A184">
         <v>293826.40000000002</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2">
       <c r="A185">
         <v>335541.40000000002</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2">
       <c r="A186">
         <v>349161.4</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2">
       <c r="A187">
         <v>357809.4</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2">
       <c r="A188">
         <v>411474.6</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2">
       <c r="A189">
         <v>413999.4</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2">
       <c r="A190">
         <v>431943.4</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2">
       <c r="A191">
         <v>485916.4</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2">
       <c r="A192">
         <v>68909.100000000006</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2">
       <c r="A193">
         <v>243230.17</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2">
       <c r="A194">
         <v>262724.09999999998</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2">
       <c r="A195">
         <v>504728.4</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2">
       <c r="A196">
         <v>526227.4</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2">
       <c r="A197">
         <v>326298.3</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2">
       <c r="A198">
         <v>367737.4</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2">
       <c r="A199">
         <v>502025.5</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2">
       <c r="A200">
         <v>246197.19</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2">
       <c r="A201">
         <v>882.1</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2">
       <c r="A202">
         <v>891.1</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2">
       <c r="A203">
         <v>273121.09999999998</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2">
       <c r="A204">
         <v>335543.59999999998</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2">
       <c r="A205">
         <v>525897.4</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2">
       <c r="A206">
         <v>387093.4</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2">
       <c r="A207">
         <v>290397.13</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2">
       <c r="A208">
         <v>217.1</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:2">
       <c r="A209">
         <v>85962.1</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:2">
       <c r="A210">
         <v>192222.1</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:2">
       <c r="A211">
         <v>235279.1</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2">
       <c r="A212">
         <v>306254.09999999998</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2">
       <c r="A213">
         <v>306263.09999999998</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2">
       <c r="A214">
         <v>306264.09999999998</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2">
       <c r="A215">
         <v>360104.4</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:2">
       <c r="A216">
         <v>360105.6</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2">
       <c r="A217">
         <v>360106.5</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:2">
       <c r="A218">
         <v>360107.5</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:2">
       <c r="A219">
         <v>382638.8</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:2">
       <c r="A220">
         <v>525898.4</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:2">
       <c r="A221">
         <v>706433.3</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:2">
       <c r="A222">
         <v>469599.3</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:2">
       <c r="A223">
         <v>519441.4</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:2">
       <c r="A224">
         <v>354.1</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:2">
       <c r="A225">
         <v>40324.1</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:2">
       <c r="A226">
         <v>62977.3</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2">
       <c r="A227">
         <v>76869.3</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:2">
       <c r="A228">
         <v>87626.3</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2">
       <c r="A229">
         <v>167879.3</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2">
       <c r="A230">
         <v>171440.1</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2">
       <c r="A231">
         <v>190485.1</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2">
       <c r="A232">
         <v>205918.4</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2">
       <c r="A233">
         <v>205922.3</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2">
       <c r="A234">
         <v>208963.3</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:2">
       <c r="A235">
         <v>221988.1</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2">
       <c r="A236">
         <v>233412.1</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2">
       <c r="A237">
         <v>243159.3</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2">
       <c r="A238">
         <v>243233.4</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2">
       <c r="A239">
         <v>283942.3</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2">
       <c r="A240">
         <v>290398.40000000002</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2">
       <c r="A241">
         <v>291331.3</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2">
       <c r="A242">
         <v>312309.3</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2">
       <c r="A243">
         <v>314275.3</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2">
       <c r="A244">
         <v>314276.3</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:2">
       <c r="A245">
         <v>314282.3</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:2">
       <c r="A246">
         <v>314283.3</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:2">
       <c r="A247">
         <v>314288.3</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2">
       <c r="A248">
         <v>316275.90000000002</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:2">
       <c r="A249">
         <v>317025.3</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:2">
       <c r="A250">
         <v>326442.40000000002</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:2">
       <c r="A251">
         <v>342610.3</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:2">
       <c r="A252">
         <v>349521.5</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:2">
       <c r="A253">
         <v>351348.5</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:2">
       <c r="A254">
         <v>357804.5</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:2">
       <c r="A255">
         <v>380703.5</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:2">
       <c r="A256">
         <v>382245.6</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:2">
       <c r="A257">
         <v>384676.6</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:2">
       <c r="A258">
         <v>399739.6</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:2">
       <c r="A259">
         <v>400667.4</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:2">
       <c r="A260">
         <v>400668.6</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:2">
       <c r="A261">
         <v>484022.4</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:2">
       <c r="A262">
         <v>498211.3</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:2">
       <c r="A263">
         <v>523791.4</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:2">
       <c r="A264">
         <v>584.1</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:2">
       <c r="A265">
         <v>615.1</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:2">
       <c r="A266">
         <v>60480.160000000003</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:2">
       <c r="A267">
         <v>94122.5</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:2">
       <c r="A268">
         <v>211586.1</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:2">
       <c r="A269">
         <v>272620.3</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:2">
       <c r="A270">
         <v>298386.09999999998</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:2">
       <c r="A271">
         <v>318161.14</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:2">
       <c r="A272">
         <v>319224.13</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:2">
       <c r="A273">
         <v>326297.7</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:2">
       <c r="A274">
         <v>392500.3</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:2">
       <c r="A275">
         <v>398579.3</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:2">
       <c r="A276">
         <v>399599.3</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:2">
       <c r="A277">
         <v>425104.3</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:2">
       <c r="A278">
         <v>458817.3</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:2">
       <c r="A279">
         <v>546273.30000000005</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:2">
       <c r="A280">
         <v>866778.4</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:2">
       <c r="A281">
         <v>1048260.3</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:2">
       <c r="A282">
         <v>63737.4</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:2">
       <c r="A283">
         <v>103690.1</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:2">
       <c r="A284">
         <v>993516.3</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:2">
       <c r="A285">
         <v>189518.1</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:2">
       <c r="A286">
         <v>12149.1</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:2">
       <c r="A287">
         <v>273075.09999999998</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:2">
       <c r="A288">
         <v>178306.1</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:2">
       <c r="A289">
         <v>272557.09999999998</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:2">
       <c r="A290">
         <v>399549.6</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:2">
       <c r="A291">
         <v>243274.1</v>
       </c>

</xml_diff>

<commit_message>
handeling case of single genome set in predict
</commit_message>
<xml_diff>
--- a/data/RealData/full_genomeid_classification.xlsx
+++ b/data/RealData/full_genomeid_classification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagoyal/Documents/kb_genomeclassification/data/RealData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D284CA-41A3-0643-8E65-63949B578C9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AE2F7E-D178-7344-A2BC-FC5A13C4C23D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="5820" windowWidth="25440" windowHeight="15000" xr2:uid="{9D33719E-AF2C-C846-B800-8BB48A352A14}"/>
+    <workbookView xWindow="1220" yWindow="5480" windowWidth="25440" windowHeight="15000" xr2:uid="{9D33719E-AF2C-C846-B800-8BB48A352A14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,12 +394,12 @@
   <dimension ref="A1:B291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>